<commit_message>
Versión final de rodolfoxp
</commit_message>
<xml_diff>
--- a/doc/retrospectiva.xlsx
+++ b/doc/retrospectiva.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Día 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Día 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
-  <si>
-    <t>Buenas</t>
-  </si>
-  <si>
-    <t>Malas</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+  <si>
+    <t>Positivo</t>
+  </si>
+  <si>
+    <t>Mejorable</t>
   </si>
   <si>
     <t>Acciones</t>
@@ -111,6 +112,33 @@
   </si>
   <si>
     <t>Hace calor</t>
+  </si>
+  <si>
+    <t>100% terminada la gestión del usuario</t>
+  </si>
+  <si>
+    <t>Pair-programming</t>
+  </si>
+  <si>
+    <t>El navegador ir pensando las clases</t>
+  </si>
+  <si>
+    <t>Aplicación de peer-expert / expert-review</t>
+  </si>
+  <si>
+    <t>Comunicación de los “pares” con el resto</t>
+  </si>
+  <si>
+    <t>Aplicación de TDD (obliga pensar el para qué de las cosas)</t>
+  </si>
+  <si>
+    <t>Tiene que haber sinergia en la pareja</t>
+  </si>
+  <si>
+    <t>Sensación de seguridad</t>
+  </si>
+  <si>
+    <t>Desvío del objetivo por temas de configuración</t>
   </si>
 </sst>
 </file>
@@ -208,8 +236,8 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A12:B24 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -358,4 +386,91 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>